<commit_message>
Changed variance scaling off for PLSR. removed the algorithm for mean centering as it is done when instantiating PLSR from sklearn.
</commit_message>
<xml_diff>
--- a/output_dil+infogest_mir_maltose_all.xlsx
+++ b/output_dil+infogest_mir_maltose_all.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PhD\2nd_year\Analysis\python_scripts\Regression\mir_plsr_maltose_dil+infogest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\PHDVIS1-A5368\PhD\2nd_year\Analysis\python_scripts\Regression\mir_plsr_maltose_dil+infogest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C2693-1284-4C54-96ED-8835FEEDC996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B61F8D-6EEF-47A1-98CA-A6A331BBA488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="descriptive_stats" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">calibration_stats_sn!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">calibration_stats_turbid!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -539,7 +540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -577,10 +580,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -589,68 +592,68 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H2">
-        <v>0.97863291260440066</v>
+        <v>0.94485900467104744</v>
       </c>
       <c r="I2">
-        <v>464.40119713640479</v>
+        <v>746.03287890952618</v>
       </c>
       <c r="J2">
-        <v>0.92213321318152652</v>
+        <v>0.92824567604636077</v>
       </c>
       <c r="K2">
-        <v>886.53685416780729</v>
+        <v>851.02967877661956</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H3">
-        <v>0.98748596275052269</v>
+        <v>0.94773960380139832</v>
       </c>
       <c r="I3">
-        <v>355.40160855393748</v>
+        <v>726.28490235457298</v>
       </c>
       <c r="J3">
-        <v>0.93346269475669186</v>
+        <v>0.91908155029347749</v>
       </c>
       <c r="K3">
-        <v>819.50813948079417</v>
+        <v>903.7419549090215</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -659,42 +662,42 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4">
-        <v>0.98868451827201953</v>
+        <v>0.94985303112642794</v>
       </c>
       <c r="I4">
-        <v>337.95368885715737</v>
+        <v>711.44775135685279</v>
       </c>
       <c r="J4">
-        <v>0.92118688761669354</v>
+        <v>0.92673637062469616</v>
       </c>
       <c r="K4">
-        <v>891.90768632943741</v>
+        <v>859.93352798822241</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -703,33 +706,33 @@
         <v>15</v>
       </c>
       <c r="H5">
-        <v>0.98928118741631876</v>
+        <v>0.95056373825218832</v>
       </c>
       <c r="I5">
-        <v>328.92282085555053</v>
+        <v>706.38827001277116</v>
       </c>
       <c r="J5">
-        <v>0.92528320644853168</v>
+        <v>0.93405692961105291</v>
       </c>
       <c r="K5">
-        <v>868.41992715903791</v>
+        <v>815.84047915175961</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -738,59 +741,59 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>0.98438357026783674</v>
+        <v>0.95071588711569832</v>
       </c>
       <c r="I6">
-        <v>397.01923033737268</v>
+        <v>705.30041475814051</v>
       </c>
       <c r="J6">
-        <v>0.9198709965869819</v>
+        <v>0.92793677439004574</v>
       </c>
       <c r="K6">
-        <v>899.32266356530749</v>
+        <v>852.8595486818549</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H7">
-        <v>0.96284327901236877</v>
+        <v>0.95142470905593235</v>
       </c>
       <c r="I7">
-        <v>612.4058886860397</v>
+        <v>700.21010293996858</v>
       </c>
       <c r="J7">
-        <v>0.914065950640503</v>
+        <v>0.92387346947790605</v>
       </c>
       <c r="K7">
-        <v>931.32938502396462</v>
+        <v>876.57420403134211</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -799,138 +802,138 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
       <c r="G8">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H8">
-        <v>0.97324612241791664</v>
+        <v>0.95174082696803175</v>
       </c>
       <c r="I8">
-        <v>519.65371353824457</v>
+        <v>697.92797295864159</v>
       </c>
       <c r="J8">
-        <v>0.91426383171780501</v>
+        <v>0.93254688398420282</v>
       </c>
       <c r="K8">
-        <v>930.25647691190977</v>
+        <v>825.12866698198206</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H9">
-        <v>0.98582589902166795</v>
+        <v>0.95397988702718328</v>
       </c>
       <c r="I9">
-        <v>378.24084807223318</v>
+        <v>681.54495543592361</v>
       </c>
       <c r="J9">
-        <v>0.92455540051099394</v>
+        <v>0.93510002872322051</v>
       </c>
       <c r="K9">
-        <v>872.63925620088628</v>
+        <v>809.36220414878392</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H10">
-        <v>0.98338035799741863</v>
+        <v>0.95599717623331348</v>
       </c>
       <c r="I10">
-        <v>409.573170212577</v>
+        <v>666.43982391111319</v>
       </c>
       <c r="J10">
-        <v>0.91515377014759314</v>
+        <v>0.94207357305349315</v>
       </c>
       <c r="K10">
-        <v>925.41586795089665</v>
+        <v>764.6435647740584</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H11">
-        <v>0.98589761817716381</v>
+        <v>0.95607673079896527</v>
       </c>
       <c r="I11">
-        <v>377.28270913030548</v>
+        <v>665.83710900112339</v>
       </c>
       <c r="J11">
-        <v>0.92189061147389539</v>
+        <v>0.93997921894942171</v>
       </c>
       <c r="K11">
-        <v>887.91682695069687</v>
+        <v>778.34383293805877</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -939,42 +942,42 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H12">
-        <v>0.97698456556530733</v>
+        <v>0.95616618104329321</v>
       </c>
       <c r="I12">
-        <v>481.98137454109519</v>
+        <v>665.15877098827491</v>
       </c>
       <c r="J12">
-        <v>0.90276445665752514</v>
+        <v>0.94218669441541725</v>
       </c>
       <c r="K12">
-        <v>990.67953146524997</v>
+        <v>763.89658454108815</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -983,21 +986,21 @@
         <v>15</v>
       </c>
       <c r="H13">
-        <v>0.9863589623397343</v>
+        <v>0.95703518872731741</v>
       </c>
       <c r="I13">
-        <v>371.0601974827382</v>
+        <v>658.53236116656933</v>
       </c>
       <c r="J13">
-        <v>0.92029460292665655</v>
+        <v>0.94572190164631997</v>
       </c>
       <c r="K13">
-        <v>896.94235437285579</v>
+        <v>740.17255749557251</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
@@ -1009,65 +1012,65 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
       <c r="G14">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H14">
-        <v>0.96311538448700373</v>
+        <v>0.957407022380244</v>
       </c>
       <c r="I14">
-        <v>610.15938798886543</v>
+        <v>655.67657548407078</v>
       </c>
       <c r="J14">
-        <v>0.92527614191467322</v>
+        <v>0.92966614228098077</v>
       </c>
       <c r="K14">
-        <v>868.46098109535626</v>
+        <v>842.56397570693775</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15">
-        <v>0.957407022380244</v>
+        <v>0.95749885282904401</v>
       </c>
       <c r="I15">
-        <v>655.67657548407078</v>
+        <v>654.96937483318368</v>
       </c>
       <c r="J15">
-        <v>0.92966614228098077</v>
+        <v>0.94877044567735469</v>
       </c>
       <c r="K15">
-        <v>842.56397570693775</v>
+        <v>719.0862032851004</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -1076,10 +1079,10 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -1088,21 +1091,21 @@
         <v>15</v>
       </c>
       <c r="H16">
-        <v>0.95853396497843091</v>
+        <v>0.95822705513581174</v>
       </c>
       <c r="I16">
-        <v>646.94434720167442</v>
+        <v>649.33410479104725</v>
       </c>
       <c r="J16">
-        <v>0.93084842985998972</v>
+        <v>0.88348472273597234</v>
       </c>
       <c r="K16">
-        <v>835.45236005108097</v>
+        <v>1084.456419423635</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -1114,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -1123,30 +1126,30 @@
         <v>15</v>
       </c>
       <c r="H17">
-        <v>0.95142470905593235</v>
+        <v>0.95853396497843091</v>
       </c>
       <c r="I17">
-        <v>700.21010293996858</v>
+        <v>646.94434720167442</v>
       </c>
       <c r="J17">
-        <v>0.92387346947790605</v>
+        <v>0.93084842985998972</v>
       </c>
       <c r="K17">
-        <v>876.57420403134211</v>
+        <v>835.45236005108097</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <v>31</v>
@@ -1158,21 +1161,21 @@
         <v>15</v>
       </c>
       <c r="H18">
-        <v>0.94985303112642794</v>
+        <v>0.95854153928572017</v>
       </c>
       <c r="I18">
-        <v>711.44775135685279</v>
+        <v>646.88525812947591</v>
       </c>
       <c r="J18">
-        <v>0.92673637062469616</v>
+        <v>0.94497815652328188</v>
       </c>
       <c r="K18">
-        <v>859.93352798822241</v>
+        <v>745.22640750759263</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
@@ -1184,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="E19">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -1193,21 +1196,21 @@
         <v>15</v>
       </c>
       <c r="H19">
-        <v>0.95822705513581174</v>
+        <v>0.96070213923289116</v>
       </c>
       <c r="I19">
-        <v>649.33410479104725</v>
+        <v>629.80357599994409</v>
       </c>
       <c r="J19">
-        <v>0.88348472273597234</v>
+        <v>0.93561584359226602</v>
       </c>
       <c r="K19">
-        <v>1084.456419423635</v>
+        <v>806.13944547385074</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -1219,7 +1222,7 @@
         <v>2</v>
       </c>
       <c r="E20">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F20">
         <v>2</v>
@@ -1228,21 +1231,21 @@
         <v>15</v>
       </c>
       <c r="H20">
-        <v>0.96145293937653209</v>
+        <v>0.96086410548529755</v>
       </c>
       <c r="I20">
-        <v>623.75824723119069</v>
+        <v>628.50436726972237</v>
       </c>
       <c r="J20">
-        <v>0.91161121882111518</v>
+        <v>0.9388218559609619</v>
       </c>
       <c r="K20">
-        <v>944.53757638897685</v>
+        <v>785.81228892420791</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1254,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="E21">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -1263,21 +1266,21 @@
         <v>15</v>
       </c>
       <c r="H21">
-        <v>0.96419271913120619</v>
+        <v>0.96145293937653209</v>
       </c>
       <c r="I21">
-        <v>601.18251209630682</v>
+        <v>623.75824723119069</v>
       </c>
       <c r="J21">
-        <v>0.93122493839057496</v>
+        <v>0.91161121882111518</v>
       </c>
       <c r="K21">
-        <v>833.17486821275543</v>
+        <v>944.53757638897685</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -1289,7 +1292,7 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -1298,24 +1301,24 @@
         <v>15</v>
       </c>
       <c r="H22">
-        <v>0.96628982228294902</v>
+        <v>0.96233893807402004</v>
       </c>
       <c r="I22">
-        <v>583.31237278523338</v>
+        <v>616.54807797463479</v>
       </c>
       <c r="J22">
-        <v>0.94280382504017823</v>
+        <v>0.9387452905093836</v>
       </c>
       <c r="K22">
-        <v>759.8085221969485</v>
+        <v>786.30386365866252</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -1324,30 +1327,30 @@
         <v>2</v>
       </c>
       <c r="E23">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="G23">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H23">
-        <v>0.96070213923289116</v>
+        <v>0.96284327901236877</v>
       </c>
       <c r="I23">
-        <v>629.80357599994409</v>
+        <v>612.4058886860397</v>
       </c>
       <c r="J23">
-        <v>0.93561584359226602</v>
+        <v>0.914065950640503</v>
       </c>
       <c r="K23">
-        <v>806.13944547385074</v>
+        <v>931.32938502396462</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
@@ -1356,10 +1359,10 @@
         <v>21</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -1368,21 +1371,21 @@
         <v>15</v>
       </c>
       <c r="H24">
-        <v>0.96233893807402004</v>
+        <v>0.96311538448700373</v>
       </c>
       <c r="I24">
-        <v>616.54807797463479</v>
+        <v>610.15938798886543</v>
       </c>
       <c r="J24">
-        <v>0.9387452905093836</v>
+        <v>0.92527614191467322</v>
       </c>
       <c r="K24">
-        <v>786.30386365866252</v>
+        <v>868.46098109535626</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
@@ -1394,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="E25">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -1403,33 +1406,33 @@
         <v>15</v>
       </c>
       <c r="H25">
-        <v>0.96086410548529755</v>
+        <v>0.96419271913120619</v>
       </c>
       <c r="I25">
-        <v>628.50436726972237</v>
+        <v>601.18251209630682</v>
       </c>
       <c r="J25">
-        <v>0.9388218559609619</v>
+        <v>0.93122493839057496</v>
       </c>
       <c r="K25">
-        <v>785.81228892420791</v>
+        <v>833.17486821275543</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
         <v>21</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F26">
         <v>2</v>
@@ -1438,30 +1441,30 @@
         <v>15</v>
       </c>
       <c r="H26">
-        <v>0.95397988702718328</v>
+        <v>0.96628982228294902</v>
       </c>
       <c r="I26">
-        <v>681.54495543592361</v>
+        <v>583.31237278523338</v>
       </c>
       <c r="J26">
-        <v>0.93510002872322051</v>
+        <v>0.94280382504017823</v>
       </c>
       <c r="K26">
-        <v>809.36220414878392</v>
+        <v>759.8085221969485</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>15</v>
@@ -1470,62 +1473,62 @@
         <v>2</v>
       </c>
       <c r="G27">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H27">
-        <v>0.95607673079896527</v>
+        <v>0.97324612241791664</v>
       </c>
       <c r="I27">
-        <v>665.83710900112339</v>
+        <v>519.65371353824457</v>
       </c>
       <c r="J27">
-        <v>0.93997921894942171</v>
+        <v>0.91426383171780501</v>
       </c>
       <c r="K27">
-        <v>778.34383293805877</v>
+        <v>930.25647691190977</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
         <v>21</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F28">
         <v>2</v>
       </c>
       <c r="G28">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H28">
-        <v>0.95599717623331348</v>
+        <v>0.97698456556530733</v>
       </c>
       <c r="I28">
-        <v>666.43982391111319</v>
+        <v>481.98137454109519</v>
       </c>
       <c r="J28">
-        <v>0.94207357305349315</v>
+        <v>0.90276445665752514</v>
       </c>
       <c r="K28">
-        <v>764.6435647740584</v>
+        <v>990.67953146524997</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
         <v>21</v>
@@ -1534,77 +1537,77 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
       <c r="G29">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H29">
-        <v>0.94485900467104744</v>
+        <v>0.97863291260440066</v>
       </c>
       <c r="I29">
-        <v>746.03287890952618</v>
+        <v>464.40119713640479</v>
       </c>
       <c r="J29">
-        <v>0.92824567604636077</v>
+        <v>0.92213321318152652</v>
       </c>
       <c r="K29">
-        <v>851.02967877661956</v>
+        <v>886.53685416780729</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
         <v>21</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F30">
         <v>2</v>
       </c>
       <c r="G30">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H30">
-        <v>0.95703518872731741</v>
+        <v>0.98338035799741863</v>
       </c>
       <c r="I30">
-        <v>658.53236116656933</v>
+        <v>409.573170212577</v>
       </c>
       <c r="J30">
-        <v>0.94572190164631997</v>
+        <v>0.91515377014759314</v>
       </c>
       <c r="K30">
-        <v>740.17255749557251</v>
+        <v>925.41586795089665</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
         <v>21</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -1613,24 +1616,24 @@
         <v>15</v>
       </c>
       <c r="H31">
-        <v>0.94773960380139832</v>
+        <v>0.98438357026783674</v>
       </c>
       <c r="I31">
-        <v>726.28490235457298</v>
+        <v>397.01923033737268</v>
       </c>
       <c r="J31">
-        <v>0.91908155029347749</v>
+        <v>0.9198709965869819</v>
       </c>
       <c r="K31">
-        <v>903.7419549090215</v>
+        <v>899.32266356530749</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
         <v>21</v>
@@ -1639,68 +1642,68 @@
         <v>2</v>
       </c>
       <c r="E32">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F32">
         <v>2</v>
       </c>
       <c r="G32">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H32">
-        <v>0.95071588711569832</v>
+        <v>0.98582589902166795</v>
       </c>
       <c r="I32">
-        <v>705.30041475814051</v>
+        <v>378.24084807223318</v>
       </c>
       <c r="J32">
-        <v>0.92793677439004574</v>
+        <v>0.92455540051099394</v>
       </c>
       <c r="K32">
-        <v>852.8595486818549</v>
+        <v>872.63925620088628</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33">
-        <v>21</v>
-      </c>
       <c r="F33">
         <v>2</v>
       </c>
       <c r="G33">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H33">
-        <v>0.95174082696803175</v>
+        <v>0.98589761817716381</v>
       </c>
       <c r="I33">
-        <v>697.92797295864159</v>
+        <v>377.28270913030548</v>
       </c>
       <c r="J33">
-        <v>0.93254688398420282</v>
+        <v>0.92189061147389539</v>
       </c>
       <c r="K33">
-        <v>825.12866698198206</v>
+        <v>887.91682695069687</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>21</v>
@@ -1709,7 +1712,7 @@
         <v>2</v>
       </c>
       <c r="E34">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="F34">
         <v>2</v>
@@ -1718,124 +1721,129 @@
         <v>15</v>
       </c>
       <c r="H34">
-        <v>0.95616618104329321</v>
+        <v>0.9863589623397343</v>
       </c>
       <c r="I34">
-        <v>665.15877098827491</v>
+        <v>371.0601974827382</v>
       </c>
       <c r="J34">
-        <v>0.94218669441541725</v>
+        <v>0.92029460292665655</v>
       </c>
       <c r="K34">
-        <v>763.89658454108815</v>
+        <v>896.94235437285579</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F35">
         <v>2</v>
       </c>
       <c r="G35">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H35">
-        <v>0.95854153928572017</v>
+        <v>0.98748596275052269</v>
       </c>
       <c r="I35">
-        <v>646.88525812947591</v>
+        <v>355.40160855393748</v>
       </c>
       <c r="J35">
-        <v>0.94497815652328188</v>
+        <v>0.93346269475669186</v>
       </c>
       <c r="K35">
-        <v>745.22640750759263</v>
+        <v>819.50813948079417</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
         <v>21</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F36">
         <v>2</v>
       </c>
       <c r="G36">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36">
-        <v>0.95056373825218832</v>
+        <v>0.98868451827201953</v>
       </c>
       <c r="I36">
-        <v>706.38827001277116</v>
+        <v>337.95368885715737</v>
       </c>
       <c r="J36">
-        <v>0.93405692961105291</v>
+        <v>0.92118688761669354</v>
       </c>
       <c r="K36">
-        <v>815.84047915175961</v>
+        <v>891.90768632943741</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
         <v>21</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F37">
         <v>2</v>
       </c>
       <c r="G37">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H37">
-        <v>0.95749885282904401</v>
+        <v>0.98928118741631876</v>
       </c>
       <c r="I37">
-        <v>654.96937483318368</v>
+        <v>328.92282085555053</v>
       </c>
       <c r="J37">
-        <v>0.94877044567735469</v>
+        <v>0.92528320644853168</v>
       </c>
       <c r="K37">
-        <v>719.0862032851004</v>
+        <v>868.41992715903791</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K37">
+      <sortCondition descending="1" ref="I1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1844,7 +1852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>

</xml_diff>